<commit_message>
Revised SF2 Thread & Finished eporting SF4
-Can now export all sf4 values
-sf2 thread can now remove students not enrolled yet based on Month Selected and Date Enrolled
</commit_message>
<xml_diff>
--- a/Project Files/Forms System Final/exports/jh_sf4.xlsx
+++ b/Project Files/Forms System Final/exports/jh_sf4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2118" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2202" uniqueCount="56">
   <si>
     <t>Grade Level</t>
   </si>
@@ -161,6 +161,45 @@
   </si>
   <si>
     <t>NOVEMBER</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FIDELITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fumino Ona Furahashi </t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Grade 7 Oreo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerby Estrella Paderogao </t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STRAWBERRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None None None </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UNITY</t>
   </si>
 </sst>
 </file>
@@ -1809,245 +1848,333 @@
       </c>
     </row>
     <row r="11" spans="1:39">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="66"/>
+      <c r="A11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="66" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="69" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="I11" s="67" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="J11" s="66" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="K11" s="67" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="L11" s="68" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="M11" s="66"/>
       <c r="N11" s="67"/>
       <c r="O11" s="69"/>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="69"/>
+      <c r="P11" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q11" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" s="69" t="s">
+        <v>47</v>
+      </c>
       <c r="S11" s="67"/>
       <c r="T11" s="66"/>
       <c r="U11" s="68"/>
       <c r="V11" s="66"/>
       <c r="W11" s="67"/>
       <c r="X11" s="69"/>
-      <c r="Y11" s="67"/>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="69"/>
+      <c r="Y11" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z11" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA11" s="69" t="s">
+        <v>47</v>
+      </c>
       <c r="AB11" s="67"/>
       <c r="AC11" s="66"/>
       <c r="AD11" s="68"/>
       <c r="AE11" s="66"/>
       <c r="AF11" s="67"/>
       <c r="AG11" s="69"/>
-      <c r="AH11" s="67"/>
-      <c r="AI11" s="66"/>
-      <c r="AJ11" s="69"/>
+      <c r="AH11" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI11" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ11" s="69" t="s">
+        <v>46</v>
+      </c>
       <c r="AK11" s="67"/>
       <c r="AL11" s="66"/>
       <c r="AM11" s="68"/>
     </row>
     <row r="12" spans="1:39">
       <c r="A12" s="8" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="F12" s="8" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="15"/>
+      <c r="P12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="S12" s="14"/>
       <c r="T12" s="4"/>
       <c r="U12" s="8"/>
       <c r="V12" s="4"/>
       <c r="W12" s="2"/>
       <c r="X12" s="15"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="15"/>
+      <c r="Y12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA12" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="AB12" s="14"/>
       <c r="AC12" s="4"/>
       <c r="AD12" s="8"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="15"/>
-      <c r="AH12" s="14"/>
-      <c r="AI12" s="4"/>
-      <c r="AJ12" s="15"/>
+      <c r="AH12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ12" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="AK12" s="14"/>
       <c r="AL12" s="4"/>
       <c r="AM12" s="8"/>
     </row>
     <row r="13" spans="1:39">
       <c r="A13" s="8" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="2"/>
       <c r="O13" s="15"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="15"/>
+      <c r="P13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R13" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="S13" s="14"/>
       <c r="T13" s="4"/>
       <c r="U13" s="8"/>
       <c r="V13" s="4"/>
       <c r="W13" s="2"/>
       <c r="X13" s="15"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="15"/>
+      <c r="Y13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA13" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="AB13" s="14"/>
       <c r="AC13" s="4"/>
       <c r="AD13" s="8"/>
       <c r="AE13" s="4"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="15"/>
-      <c r="AH13" s="14"/>
-      <c r="AI13" s="4"/>
-      <c r="AJ13" s="15"/>
+      <c r="AH13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ13" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="AK13" s="14"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="8"/>
     </row>
     <row r="14" spans="1:39">
       <c r="A14" s="8" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="2"/>
       <c r="O14" s="15"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="15"/>
+      <c r="P14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="S14" s="14"/>
       <c r="T14" s="4"/>
       <c r="U14" s="8"/>
       <c r="V14" s="4"/>
       <c r="W14" s="2"/>
       <c r="X14" s="15"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="15"/>
+      <c r="Y14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA14" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="AB14" s="14"/>
       <c r="AC14" s="4"/>
       <c r="AD14" s="8"/>
       <c r="AE14" s="4"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="15"/>
-      <c r="AH14" s="14"/>
-      <c r="AI14" s="4"/>
-      <c r="AJ14" s="15"/>
+      <c r="AH14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ14" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="AK14" s="14"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="8"/>

</xml_diff>